<commit_message>
Adding Lab 21 HumMod data. This one appears to be quite reasonable.
</commit_message>
<xml_diff>
--- a/21_pneumothorax/pneumothorax_data.xlsx
+++ b/21_pneumothorax/pneumothorax_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>Time</t>
   </si>
@@ -61,6 +61,36 @@
   </si>
   <si>
     <t>Respiratory Drive</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>mL/min</t>
+  </si>
+  <si>
+    <t>bpm</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>L/min</t>
+  </si>
+  <si>
+    <t>x-norm</t>
+  </si>
+  <si>
+    <t>5 minutes</t>
   </si>
 </sst>
 </file>
@@ -90,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -118,56 +148,29 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,179 +477,433 @@
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>5346</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>5309</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>4982</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>72</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>77</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A4" s="3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>75</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>69</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>91</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>47</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A6" s="3" t="s">
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>5413</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>5413</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>5345</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A7" s="3" t="s">
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>6.5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>6.4</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A8" s="3" t="s">
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>13</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>16</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A9" s="3" t="s">
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>516</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>409</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>462</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A10" s="3" t="s">
+      <c r="E9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>1.9</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2.1800000000000002</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3">
+        <v>5468</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5751</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5405</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3">
+        <v>72</v>
+      </c>
+      <c r="C17" s="3">
+        <v>74</v>
+      </c>
+      <c r="D17" s="3">
+        <v>72</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3">
+        <v>76</v>
+      </c>
+      <c r="C18" s="3">
+        <v>78</v>
+      </c>
+      <c r="D18" s="3">
+        <v>75</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3">
+        <v>7.43</v>
+      </c>
+      <c r="C19" s="3">
+        <v>7.51</v>
+      </c>
+      <c r="D19" s="3">
+        <v>7.42</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3">
+        <v>5421</v>
+      </c>
+      <c r="C20" s="3">
+        <v>5419</v>
+      </c>
+      <c r="D20" s="3">
+        <v>5751</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="C21" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="3">
+        <v>12</v>
+      </c>
+      <c r="C22" s="3">
+        <v>21.3</v>
+      </c>
+      <c r="D22" s="3">
+        <v>24</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3">
+        <v>550.9</v>
+      </c>
+      <c r="C23" s="3">
+        <v>681.1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>774.1</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="C27" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Making various changes to data
</commit_message>
<xml_diff>
--- a/21_pneumothorax/pneumothorax_data.xlsx
+++ b/21_pneumothorax/pneumothorax_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
   <si>
     <t>Time</t>
   </si>
@@ -91,13 +91,19 @@
   </si>
   <si>
     <t>5 minutes</t>
+  </si>
+  <si>
+    <t>breaths/min</t>
+  </si>
+  <si>
+    <t>% Diff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +117,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -152,11 +165,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -171,9 +196,16 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,13 +622,13 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>6.5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>6.4</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>7.8</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -617,7 +649,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1">
@@ -726,7 +758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -743,7 +775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -760,24 +792,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="3">
-        <v>7.43</v>
+        <v>93</v>
       </c>
       <c r="C19" s="3">
-        <v>7.51</v>
+        <v>43</v>
       </c>
       <c r="D19" s="3">
-        <v>7.42</v>
+        <v>49</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -794,24 +826,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>6.6</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="4">
         <v>14.5</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <v>18.600000000000001</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -825,10 +857,10 @@
         <v>24</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -845,7 +877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -862,7 +894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -879,7 +911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -896,9 +928,244 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="C27" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="6">
+        <f>ABS((B2-B16)/B2)</f>
+        <v>2.2820800598578377E-2</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" ref="C30:D30" si="0">ABS((C2-C16)/C2)</f>
+        <v>8.3254850254285181E-2</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="0"/>
+        <v>8.4905660377358486E-2</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="6">
+        <f t="shared" ref="B31:D31" si="1">ABS((B3-B17)/B3)</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="1"/>
+        <v>3.896103896103896E-2</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="1"/>
+        <v>0.16279069767441862</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="6">
+        <f t="shared" ref="B32:D32" si="2">ABS((B4-B18)/B4)</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="2"/>
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="2"/>
+        <v>0.29310344827586204</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="6">
+        <f t="shared" ref="B33:D33" si="3">ABS((B5-B19)/B5)</f>
+        <v>2.197802197802198E-2</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="3"/>
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="6">
+        <f t="shared" ref="B34:D34" si="4">ABS((B6-B20)/B6)</f>
+        <v>1.4779235174579716E-3</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1084426380934787E-3</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="4"/>
+        <v>7.5958840037418152E-2</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="6">
+        <f t="shared" ref="B35:D35" si="5">ABS((B7-B21)/B7)</f>
+        <v>1.538461538461533E-2</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="5"/>
+        <v>1.2656249999999998</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" si="5"/>
+        <v>1.3846153846153848</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="6">
+        <f t="shared" ref="B36:D36" si="6">ABS((B8-B22)/B8)</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="6"/>
+        <v>0.33125000000000004</v>
+      </c>
+      <c r="D36" s="6">
+        <f t="shared" si="6"/>
+        <v>0.41176470588235292</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="6">
+        <f t="shared" ref="B37:D37" si="7">ABS((B9-B23)/B9)</f>
+        <v>6.7635658914728641E-2</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="7"/>
+        <v>0.66528117359413208</v>
+      </c>
+      <c r="D37" s="6">
+        <f t="shared" si="7"/>
+        <v>0.67554112554112555</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="6">
+        <f t="shared" ref="B38:D38" si="8">ABS((B10-B24)/B10)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="6">
+        <f t="shared" ref="B39:D39" si="9">ABS((B11-B25)/B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="6">
+        <f t="shared" ref="B40:D40" si="10">ABS((B12-B26)/B12)</f>
+        <v>0.10714285714285723</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="10"/>
+        <v>0.6842105263157896</v>
+      </c>
+      <c r="D40" s="6">
+        <f t="shared" si="10"/>
+        <v>0.78899082568807322</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding colorcodes to Lab 21
</commit_message>
<xml_diff>
--- a/21_pneumothorax/pneumothorax_data.xlsx
+++ b/21_pneumothorax/pneumothorax_data.xlsx
@@ -210,7 +210,50 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -502,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1176,6 +1219,15 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B30:D40">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>